<commit_message>
(+) export nllai mhs to excel method
</commit_message>
<xml_diff>
--- a/resources/assets/templates/Template Ekspor Data Nilai.xlsx
+++ b/resources/assets/templates/Template Ekspor Data Nilai.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wahyu Purnomo Ady\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Skripsi\kkn-undip-be\resources\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E966F914-BE09-4147-B18B-981886CF9F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF830F72-ADFA-46A8-956F-B3BC60748E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8589C051-7EB9-4D60-A1F6-9A43CD444282}"/>
   </bookViews>
@@ -359,36 +359,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -400,6 +370,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,14 +717,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7039EB-C354-4F70-9B78-EB5375FC3A04}">
   <dimension ref="A1:T810"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="23" style="2" customWidth="1"/>
@@ -748,115 +748,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
     </row>
     <row r="5" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="28" t="s">
@@ -865,31 +865,31 @@
       <c r="F6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="30" t="s">
         <v>16</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -909,28 +909,28 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="22" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="24"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="33"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -948,11 +948,11 @@
       <c r="M8" s="7"/>
       <c r="N8" s="11"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="33"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
@@ -970,11 +970,11 @@
       <c r="M9" s="7"/>
       <c r="N9" s="11"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="33"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
@@ -992,11 +992,11 @@
       <c r="M10" s="7"/>
       <c r="N10" s="11"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="33"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="23"/>
     </row>
     <row r="11" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
@@ -1014,11 +1014,11 @@
       <c r="M11" s="7"/>
       <c r="N11" s="11"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="33"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="23"/>
     </row>
     <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -1036,11 +1036,11 @@
       <c r="M12" s="7"/>
       <c r="N12" s="11"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="33"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="23"/>
     </row>
     <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
@@ -1058,11 +1058,11 @@
       <c r="M13" s="7"/>
       <c r="N13" s="11"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="33"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="23"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -1080,11 +1080,11 @@
       <c r="M14" s="7"/>
       <c r="N14" s="11"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="33"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
@@ -1102,11 +1102,11 @@
       <c r="M15" s="7"/>
       <c r="N15" s="11"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="33"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="23"/>
     </row>
     <row r="16" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
@@ -1124,11 +1124,11 @@
       <c r="M16" s="7"/>
       <c r="N16" s="11"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="33"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
@@ -1146,11 +1146,11 @@
       <c r="M17" s="7"/>
       <c r="N17" s="11"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="33"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="23"/>
     </row>
     <row r="18" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
@@ -1168,11 +1168,11 @@
       <c r="M18" s="7"/>
       <c r="N18" s="11"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="33"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="23"/>
     </row>
     <row r="19" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
@@ -1190,11 +1190,11 @@
       <c r="M19" s="7"/>
       <c r="N19" s="11"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="33"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="23"/>
     </row>
     <row r="20" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -1212,11 +1212,11 @@
       <c r="M20" s="7"/>
       <c r="N20" s="11"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="33"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="23"/>
     </row>
     <row r="21" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
@@ -1234,11 +1234,11 @@
       <c r="M21" s="7"/>
       <c r="N21" s="11"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="33"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="23"/>
     </row>
     <row r="22" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
@@ -1256,11 +1256,11 @@
       <c r="M22" s="7"/>
       <c r="N22" s="11"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="33"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="23"/>
     </row>
     <row r="23" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
@@ -1278,11 +1278,11 @@
       <c r="M23" s="7"/>
       <c r="N23" s="11"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="33"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="23"/>
     </row>
     <row r="24" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
@@ -1300,11 +1300,11 @@
       <c r="M24" s="7"/>
       <c r="N24" s="11"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="33"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="23"/>
     </row>
     <row r="25" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
@@ -1322,11 +1322,11 @@
       <c r="M25" s="7"/>
       <c r="N25" s="11"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="32"/>
-      <c r="T25" s="33"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="23"/>
     </row>
     <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
@@ -1344,11 +1344,11 @@
       <c r="M26" s="7"/>
       <c r="N26" s="11"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="32"/>
-      <c r="T26" s="33"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="23"/>
     </row>
     <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
@@ -1366,11 +1366,11 @@
       <c r="M27" s="7"/>
       <c r="N27" s="11"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="32"/>
-      <c r="T27" s="33"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="23"/>
     </row>
     <row r="28" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
@@ -1388,11 +1388,11 @@
       <c r="M28" s="7"/>
       <c r="N28" s="11"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="33"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="23"/>
     </row>
     <row r="29" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
@@ -1410,11 +1410,11 @@
       <c r="M29" s="7"/>
       <c r="N29" s="11"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="31"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="33"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="23"/>
     </row>
     <row r="30" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
@@ -1432,11 +1432,11 @@
       <c r="M30" s="7"/>
       <c r="N30" s="11"/>
       <c r="O30" s="10"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="32"/>
-      <c r="T30" s="33"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
@@ -1454,11 +1454,11 @@
       <c r="M31" s="7"/>
       <c r="N31" s="11"/>
       <c r="O31" s="10"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="31"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="33"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="23"/>
     </row>
     <row r="32" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
@@ -1476,11 +1476,11 @@
       <c r="M32" s="7"/>
       <c r="N32" s="11"/>
       <c r="O32" s="10"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="32"/>
-      <c r="T32" s="33"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="23"/>
     </row>
     <row r="33" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
@@ -1498,11 +1498,11 @@
       <c r="M33" s="7"/>
       <c r="N33" s="11"/>
       <c r="O33" s="10"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="31"/>
-      <c r="S33" s="32"/>
-      <c r="T33" s="33"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="23"/>
     </row>
     <row r="34" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
@@ -1520,11 +1520,11 @@
       <c r="M34" s="7"/>
       <c r="N34" s="11"/>
       <c r="O34" s="10"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="33"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="23"/>
     </row>
     <row r="35" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -1542,11 +1542,11 @@
       <c r="M35" s="7"/>
       <c r="N35" s="11"/>
       <c r="O35" s="10"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="31"/>
-      <c r="S35" s="32"/>
-      <c r="T35" s="33"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="23"/>
     </row>
     <row r="36" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
@@ -1564,11 +1564,11 @@
       <c r="M36" s="7"/>
       <c r="N36" s="11"/>
       <c r="O36" s="10"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="31"/>
-      <c r="S36" s="32"/>
-      <c r="T36" s="33"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="23"/>
     </row>
     <row r="37" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
@@ -1586,11 +1586,11 @@
       <c r="M37" s="7"/>
       <c r="N37" s="11"/>
       <c r="O37" s="10"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="32"/>
-      <c r="T37" s="33"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="23"/>
     </row>
     <row r="38" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
@@ -1608,11 +1608,11 @@
       <c r="M38" s="7"/>
       <c r="N38" s="11"/>
       <c r="O38" s="10"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="31"/>
-      <c r="S38" s="32"/>
-      <c r="T38" s="33"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="23"/>
     </row>
     <row r="39" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
@@ -1630,11 +1630,11 @@
       <c r="M39" s="7"/>
       <c r="N39" s="11"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="31"/>
-      <c r="S39" s="32"/>
-      <c r="T39" s="33"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="23"/>
     </row>
     <row r="40" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
@@ -1652,11 +1652,11 @@
       <c r="M40" s="7"/>
       <c r="N40" s="11"/>
       <c r="O40" s="10"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="31"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="33"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="23"/>
     </row>
     <row r="41" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
@@ -1674,11 +1674,11 @@
       <c r="M41" s="7"/>
       <c r="N41" s="11"/>
       <c r="O41" s="10"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="31"/>
-      <c r="S41" s="32"/>
-      <c r="T41" s="33"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="23"/>
     </row>
     <row r="42" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
@@ -1696,11 +1696,11 @@
       <c r="M42" s="7"/>
       <c r="N42" s="11"/>
       <c r="O42" s="10"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="30"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="32"/>
-      <c r="T42" s="33"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="23"/>
     </row>
     <row r="43" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
@@ -1718,11 +1718,11 @@
       <c r="M43" s="7"/>
       <c r="N43" s="11"/>
       <c r="O43" s="10"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="32"/>
-      <c r="T43" s="33"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="23"/>
     </row>
     <row r="44" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
@@ -1740,11 +1740,11 @@
       <c r="M44" s="7"/>
       <c r="N44" s="11"/>
       <c r="O44" s="10"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="31"/>
-      <c r="S44" s="32"/>
-      <c r="T44" s="33"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="23"/>
     </row>
     <row r="45" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
@@ -1762,11 +1762,11 @@
       <c r="M45" s="7"/>
       <c r="N45" s="11"/>
       <c r="O45" s="10"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="30"/>
-      <c r="R45" s="31"/>
-      <c r="S45" s="32"/>
-      <c r="T45" s="33"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="23"/>
     </row>
     <row r="46" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
@@ -1784,11 +1784,11 @@
       <c r="M46" s="7"/>
       <c r="N46" s="11"/>
       <c r="O46" s="10"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="31"/>
-      <c r="S46" s="32"/>
-      <c r="T46" s="33"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="23"/>
     </row>
     <row r="47" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
@@ -1806,11 +1806,11 @@
       <c r="M47" s="7"/>
       <c r="N47" s="11"/>
       <c r="O47" s="10"/>
-      <c r="P47" s="30"/>
-      <c r="Q47" s="30"/>
-      <c r="R47" s="31"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="33"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="23"/>
     </row>
     <row r="48" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
@@ -1828,11 +1828,11 @@
       <c r="M48" s="7"/>
       <c r="N48" s="11"/>
       <c r="O48" s="10"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="31"/>
-      <c r="S48" s="32"/>
-      <c r="T48" s="33"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="21"/>
+      <c r="S48" s="22"/>
+      <c r="T48" s="23"/>
     </row>
     <row r="49" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
@@ -1850,11 +1850,11 @@
       <c r="M49" s="7"/>
       <c r="N49" s="11"/>
       <c r="O49" s="10"/>
-      <c r="P49" s="30"/>
-      <c r="Q49" s="30"/>
-      <c r="R49" s="31"/>
-      <c r="S49" s="32"/>
-      <c r="T49" s="33"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="23"/>
     </row>
     <row r="50" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
@@ -1872,11 +1872,11 @@
       <c r="M50" s="7"/>
       <c r="N50" s="11"/>
       <c r="O50" s="10"/>
-      <c r="P50" s="30"/>
-      <c r="Q50" s="30"/>
-      <c r="R50" s="31"/>
-      <c r="S50" s="32"/>
-      <c r="T50" s="33"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="21"/>
+      <c r="S50" s="22"/>
+      <c r="T50" s="23"/>
     </row>
     <row r="51" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
@@ -1894,11 +1894,11 @@
       <c r="M51" s="7"/>
       <c r="N51" s="11"/>
       <c r="O51" s="10"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="31"/>
-      <c r="S51" s="32"/>
-      <c r="T51" s="33"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="22"/>
+      <c r="T51" s="23"/>
     </row>
     <row r="52" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
@@ -1916,11 +1916,11 @@
       <c r="M52" s="7"/>
       <c r="N52" s="11"/>
       <c r="O52" s="10"/>
-      <c r="P52" s="30"/>
-      <c r="Q52" s="30"/>
-      <c r="R52" s="31"/>
-      <c r="S52" s="32"/>
-      <c r="T52" s="33"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="21"/>
+      <c r="S52" s="22"/>
+      <c r="T52" s="23"/>
     </row>
     <row r="53" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
@@ -1938,11 +1938,11 @@
       <c r="M53" s="7"/>
       <c r="N53" s="11"/>
       <c r="O53" s="10"/>
-      <c r="P53" s="30"/>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="31"/>
-      <c r="S53" s="32"/>
-      <c r="T53" s="33"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="20"/>
+      <c r="R53" s="21"/>
+      <c r="S53" s="22"/>
+      <c r="T53" s="23"/>
     </row>
     <row r="54" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
@@ -1960,11 +1960,11 @@
       <c r="M54" s="7"/>
       <c r="N54" s="11"/>
       <c r="O54" s="10"/>
-      <c r="P54" s="30"/>
-      <c r="Q54" s="30"/>
-      <c r="R54" s="31"/>
-      <c r="S54" s="32"/>
-      <c r="T54" s="33"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="21"/>
+      <c r="S54" s="22"/>
+      <c r="T54" s="23"/>
     </row>
     <row r="55" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
@@ -1982,11 +1982,11 @@
       <c r="M55" s="7"/>
       <c r="N55" s="11"/>
       <c r="O55" s="10"/>
-      <c r="P55" s="30"/>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="31"/>
-      <c r="S55" s="32"/>
-      <c r="T55" s="33"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="21"/>
+      <c r="S55" s="22"/>
+      <c r="T55" s="23"/>
     </row>
     <row r="56" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
@@ -2004,11 +2004,11 @@
       <c r="M56" s="7"/>
       <c r="N56" s="11"/>
       <c r="O56" s="10"/>
-      <c r="P56" s="30"/>
-      <c r="Q56" s="30"/>
-      <c r="R56" s="31"/>
-      <c r="S56" s="32"/>
-      <c r="T56" s="33"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="21"/>
+      <c r="S56" s="22"/>
+      <c r="T56" s="23"/>
     </row>
     <row r="57" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
@@ -2026,11 +2026,11 @@
       <c r="M57" s="7"/>
       <c r="N57" s="11"/>
       <c r="O57" s="10"/>
-      <c r="P57" s="30"/>
-      <c r="Q57" s="30"/>
-      <c r="R57" s="31"/>
-      <c r="S57" s="32"/>
-      <c r="T57" s="33"/>
+      <c r="P57" s="20"/>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="21"/>
+      <c r="S57" s="22"/>
+      <c r="T57" s="23"/>
     </row>
     <row r="58" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
@@ -2048,11 +2048,11 @@
       <c r="M58" s="7"/>
       <c r="N58" s="11"/>
       <c r="O58" s="10"/>
-      <c r="P58" s="30"/>
-      <c r="Q58" s="30"/>
-      <c r="R58" s="31"/>
-      <c r="S58" s="32"/>
-      <c r="T58" s="33"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="21"/>
+      <c r="S58" s="22"/>
+      <c r="T58" s="23"/>
     </row>
     <row r="59" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
@@ -2070,11 +2070,11 @@
       <c r="M59" s="7"/>
       <c r="N59" s="11"/>
       <c r="O59" s="10"/>
-      <c r="P59" s="30"/>
-      <c r="Q59" s="30"/>
-      <c r="R59" s="31"/>
-      <c r="S59" s="32"/>
-      <c r="T59" s="33"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="20"/>
+      <c r="R59" s="21"/>
+      <c r="S59" s="22"/>
+      <c r="T59" s="23"/>
     </row>
     <row r="60" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
@@ -2092,11 +2092,11 @@
       <c r="M60" s="7"/>
       <c r="N60" s="11"/>
       <c r="O60" s="10"/>
-      <c r="P60" s="30"/>
-      <c r="Q60" s="30"/>
-      <c r="R60" s="31"/>
-      <c r="S60" s="32"/>
-      <c r="T60" s="33"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="21"/>
+      <c r="S60" s="22"/>
+      <c r="T60" s="23"/>
     </row>
     <row r="61" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
@@ -2114,11 +2114,11 @@
       <c r="M61" s="7"/>
       <c r="N61" s="11"/>
       <c r="O61" s="10"/>
-      <c r="P61" s="30"/>
-      <c r="Q61" s="30"/>
-      <c r="R61" s="31"/>
-      <c r="S61" s="32"/>
-      <c r="T61" s="33"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="21"/>
+      <c r="S61" s="22"/>
+      <c r="T61" s="23"/>
     </row>
     <row r="62" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
@@ -2136,11 +2136,11 @@
       <c r="M62" s="7"/>
       <c r="N62" s="11"/>
       <c r="O62" s="10"/>
-      <c r="P62" s="30"/>
-      <c r="Q62" s="30"/>
-      <c r="R62" s="31"/>
-      <c r="S62" s="32"/>
-      <c r="T62" s="33"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="21"/>
+      <c r="S62" s="22"/>
+      <c r="T62" s="23"/>
     </row>
     <row r="63" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
@@ -2158,11 +2158,11 @@
       <c r="M63" s="7"/>
       <c r="N63" s="11"/>
       <c r="O63" s="10"/>
-      <c r="P63" s="30"/>
-      <c r="Q63" s="30"/>
-      <c r="R63" s="31"/>
-      <c r="S63" s="32"/>
-      <c r="T63" s="33"/>
+      <c r="P63" s="20"/>
+      <c r="Q63" s="20"/>
+      <c r="R63" s="21"/>
+      <c r="S63" s="22"/>
+      <c r="T63" s="23"/>
     </row>
     <row r="64" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
@@ -2180,11 +2180,11 @@
       <c r="M64" s="7"/>
       <c r="N64" s="11"/>
       <c r="O64" s="10"/>
-      <c r="P64" s="30"/>
-      <c r="Q64" s="30"/>
-      <c r="R64" s="31"/>
-      <c r="S64" s="32"/>
-      <c r="T64" s="33"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="21"/>
+      <c r="S64" s="22"/>
+      <c r="T64" s="23"/>
     </row>
     <row r="65" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
@@ -2202,11 +2202,11 @@
       <c r="M65" s="7"/>
       <c r="N65" s="11"/>
       <c r="O65" s="10"/>
-      <c r="P65" s="30"/>
-      <c r="Q65" s="30"/>
-      <c r="R65" s="31"/>
-      <c r="S65" s="32"/>
-      <c r="T65" s="33"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="20"/>
+      <c r="R65" s="21"/>
+      <c r="S65" s="22"/>
+      <c r="T65" s="23"/>
     </row>
     <row r="66" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
@@ -2224,11 +2224,11 @@
       <c r="M66" s="7"/>
       <c r="N66" s="11"/>
       <c r="O66" s="10"/>
-      <c r="P66" s="30"/>
-      <c r="Q66" s="30"/>
-      <c r="R66" s="31"/>
-      <c r="S66" s="32"/>
-      <c r="T66" s="33"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="21"/>
+      <c r="S66" s="22"/>
+      <c r="T66" s="23"/>
     </row>
     <row r="67" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
@@ -2246,11 +2246,11 @@
       <c r="M67" s="7"/>
       <c r="N67" s="11"/>
       <c r="O67" s="10"/>
-      <c r="P67" s="30"/>
-      <c r="Q67" s="30"/>
-      <c r="R67" s="31"/>
-      <c r="S67" s="32"/>
-      <c r="T67" s="33"/>
+      <c r="P67" s="20"/>
+      <c r="Q67" s="20"/>
+      <c r="R67" s="21"/>
+      <c r="S67" s="22"/>
+      <c r="T67" s="23"/>
     </row>
     <row r="68" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
@@ -2268,11 +2268,11 @@
       <c r="M68" s="7"/>
       <c r="N68" s="11"/>
       <c r="O68" s="10"/>
-      <c r="P68" s="30"/>
-      <c r="Q68" s="30"/>
-      <c r="R68" s="31"/>
-      <c r="S68" s="32"/>
-      <c r="T68" s="33"/>
+      <c r="P68" s="20"/>
+      <c r="Q68" s="20"/>
+      <c r="R68" s="21"/>
+      <c r="S68" s="22"/>
+      <c r="T68" s="23"/>
     </row>
     <row r="69" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
@@ -2290,11 +2290,11 @@
       <c r="M69" s="7"/>
       <c r="N69" s="11"/>
       <c r="O69" s="10"/>
-      <c r="P69" s="30"/>
-      <c r="Q69" s="30"/>
-      <c r="R69" s="31"/>
-      <c r="S69" s="32"/>
-      <c r="T69" s="33"/>
+      <c r="P69" s="20"/>
+      <c r="Q69" s="20"/>
+      <c r="R69" s="21"/>
+      <c r="S69" s="22"/>
+      <c r="T69" s="23"/>
     </row>
     <row r="70" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
@@ -2312,11 +2312,11 @@
       <c r="M70" s="7"/>
       <c r="N70" s="11"/>
       <c r="O70" s="10"/>
-      <c r="P70" s="30"/>
-      <c r="Q70" s="30"/>
-      <c r="R70" s="31"/>
-      <c r="S70" s="32"/>
-      <c r="T70" s="33"/>
+      <c r="P70" s="20"/>
+      <c r="Q70" s="20"/>
+      <c r="R70" s="21"/>
+      <c r="S70" s="22"/>
+      <c r="T70" s="23"/>
     </row>
     <row r="71" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
@@ -2334,11 +2334,11 @@
       <c r="M71" s="7"/>
       <c r="N71" s="11"/>
       <c r="O71" s="10"/>
-      <c r="P71" s="30"/>
-      <c r="Q71" s="30"/>
-      <c r="R71" s="31"/>
-      <c r="S71" s="32"/>
-      <c r="T71" s="33"/>
+      <c r="P71" s="20"/>
+      <c r="Q71" s="20"/>
+      <c r="R71" s="21"/>
+      <c r="S71" s="22"/>
+      <c r="T71" s="23"/>
     </row>
     <row r="72" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
@@ -2356,11 +2356,11 @@
       <c r="M72" s="7"/>
       <c r="N72" s="11"/>
       <c r="O72" s="10"/>
-      <c r="P72" s="30"/>
-      <c r="Q72" s="30"/>
-      <c r="R72" s="31"/>
-      <c r="S72" s="32"/>
-      <c r="T72" s="33"/>
+      <c r="P72" s="20"/>
+      <c r="Q72" s="20"/>
+      <c r="R72" s="21"/>
+      <c r="S72" s="22"/>
+      <c r="T72" s="23"/>
     </row>
     <row r="73" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
@@ -2378,11 +2378,11 @@
       <c r="M73" s="7"/>
       <c r="N73" s="11"/>
       <c r="O73" s="10"/>
-      <c r="P73" s="30"/>
-      <c r="Q73" s="30"/>
-      <c r="R73" s="31"/>
-      <c r="S73" s="32"/>
-      <c r="T73" s="33"/>
+      <c r="P73" s="20"/>
+      <c r="Q73" s="20"/>
+      <c r="R73" s="21"/>
+      <c r="S73" s="22"/>
+      <c r="T73" s="23"/>
     </row>
     <row r="74" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
@@ -2400,11 +2400,11 @@
       <c r="M74" s="7"/>
       <c r="N74" s="11"/>
       <c r="O74" s="10"/>
-      <c r="P74" s="30"/>
-      <c r="Q74" s="30"/>
-      <c r="R74" s="31"/>
-      <c r="S74" s="32"/>
-      <c r="T74" s="33"/>
+      <c r="P74" s="20"/>
+      <c r="Q74" s="20"/>
+      <c r="R74" s="21"/>
+      <c r="S74" s="22"/>
+      <c r="T74" s="23"/>
     </row>
     <row r="75" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
@@ -2422,11 +2422,11 @@
       <c r="M75" s="7"/>
       <c r="N75" s="11"/>
       <c r="O75" s="10"/>
-      <c r="P75" s="30"/>
-      <c r="Q75" s="30"/>
-      <c r="R75" s="31"/>
-      <c r="S75" s="32"/>
-      <c r="T75" s="33"/>
+      <c r="P75" s="20"/>
+      <c r="Q75" s="20"/>
+      <c r="R75" s="21"/>
+      <c r="S75" s="22"/>
+      <c r="T75" s="23"/>
     </row>
     <row r="76" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
@@ -2444,11 +2444,11 @@
       <c r="M76" s="7"/>
       <c r="N76" s="11"/>
       <c r="O76" s="10"/>
-      <c r="P76" s="30"/>
-      <c r="Q76" s="30"/>
-      <c r="R76" s="31"/>
-      <c r="S76" s="32"/>
-      <c r="T76" s="33"/>
+      <c r="P76" s="20"/>
+      <c r="Q76" s="20"/>
+      <c r="R76" s="21"/>
+      <c r="S76" s="22"/>
+      <c r="T76" s="23"/>
     </row>
     <row r="77" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
@@ -2466,11 +2466,11 @@
       <c r="M77" s="7"/>
       <c r="N77" s="11"/>
       <c r="O77" s="10"/>
-      <c r="P77" s="30"/>
-      <c r="Q77" s="30"/>
-      <c r="R77" s="31"/>
-      <c r="S77" s="32"/>
-      <c r="T77" s="33"/>
+      <c r="P77" s="20"/>
+      <c r="Q77" s="20"/>
+      <c r="R77" s="21"/>
+      <c r="S77" s="22"/>
+      <c r="T77" s="23"/>
     </row>
     <row r="78" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
@@ -2488,11 +2488,11 @@
       <c r="M78" s="7"/>
       <c r="N78" s="11"/>
       <c r="O78" s="10"/>
-      <c r="P78" s="30"/>
-      <c r="Q78" s="30"/>
-      <c r="R78" s="31"/>
-      <c r="S78" s="32"/>
-      <c r="T78" s="33"/>
+      <c r="P78" s="20"/>
+      <c r="Q78" s="20"/>
+      <c r="R78" s="21"/>
+      <c r="S78" s="22"/>
+      <c r="T78" s="23"/>
     </row>
     <row r="79" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
@@ -2510,11 +2510,11 @@
       <c r="M79" s="7"/>
       <c r="N79" s="11"/>
       <c r="O79" s="10"/>
-      <c r="P79" s="30"/>
-      <c r="Q79" s="30"/>
-      <c r="R79" s="31"/>
-      <c r="S79" s="32"/>
-      <c r="T79" s="33"/>
+      <c r="P79" s="20"/>
+      <c r="Q79" s="20"/>
+      <c r="R79" s="21"/>
+      <c r="S79" s="22"/>
+      <c r="T79" s="23"/>
     </row>
     <row r="80" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
@@ -2532,11 +2532,11 @@
       <c r="M80" s="7"/>
       <c r="N80" s="11"/>
       <c r="O80" s="10"/>
-      <c r="P80" s="30"/>
-      <c r="Q80" s="30"/>
-      <c r="R80" s="31"/>
-      <c r="S80" s="32"/>
-      <c r="T80" s="33"/>
+      <c r="P80" s="20"/>
+      <c r="Q80" s="20"/>
+      <c r="R80" s="21"/>
+      <c r="S80" s="22"/>
+      <c r="T80" s="23"/>
     </row>
     <row r="81" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
@@ -2554,11 +2554,11 @@
       <c r="M81" s="7"/>
       <c r="N81" s="11"/>
       <c r="O81" s="10"/>
-      <c r="P81" s="30"/>
-      <c r="Q81" s="30"/>
-      <c r="R81" s="31"/>
-      <c r="S81" s="32"/>
-      <c r="T81" s="33"/>
+      <c r="P81" s="20"/>
+      <c r="Q81" s="20"/>
+      <c r="R81" s="21"/>
+      <c r="S81" s="22"/>
+      <c r="T81" s="23"/>
     </row>
     <row r="82" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="16"/>
@@ -2576,11 +2576,11 @@
       <c r="M82" s="7"/>
       <c r="N82" s="11"/>
       <c r="O82" s="10"/>
-      <c r="P82" s="30"/>
-      <c r="Q82" s="30"/>
-      <c r="R82" s="31"/>
-      <c r="S82" s="32"/>
-      <c r="T82" s="33"/>
+      <c r="P82" s="20"/>
+      <c r="Q82" s="20"/>
+      <c r="R82" s="21"/>
+      <c r="S82" s="22"/>
+      <c r="T82" s="23"/>
     </row>
     <row r="83" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="16"/>
@@ -2598,11 +2598,11 @@
       <c r="M83" s="7"/>
       <c r="N83" s="11"/>
       <c r="O83" s="10"/>
-      <c r="P83" s="30"/>
-      <c r="Q83" s="30"/>
-      <c r="R83" s="31"/>
-      <c r="S83" s="32"/>
-      <c r="T83" s="33"/>
+      <c r="P83" s="20"/>
+      <c r="Q83" s="20"/>
+      <c r="R83" s="21"/>
+      <c r="S83" s="22"/>
+      <c r="T83" s="23"/>
     </row>
     <row r="84" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="16"/>
@@ -2620,11 +2620,11 @@
       <c r="M84" s="7"/>
       <c r="N84" s="11"/>
       <c r="O84" s="10"/>
-      <c r="P84" s="30"/>
-      <c r="Q84" s="30"/>
-      <c r="R84" s="31"/>
-      <c r="S84" s="32"/>
-      <c r="T84" s="33"/>
+      <c r="P84" s="20"/>
+      <c r="Q84" s="20"/>
+      <c r="R84" s="21"/>
+      <c r="S84" s="22"/>
+      <c r="T84" s="23"/>
     </row>
     <row r="85" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="16"/>
@@ -2642,11 +2642,11 @@
       <c r="M85" s="7"/>
       <c r="N85" s="11"/>
       <c r="O85" s="10"/>
-      <c r="P85" s="30"/>
-      <c r="Q85" s="30"/>
-      <c r="R85" s="31"/>
-      <c r="S85" s="32"/>
-      <c r="T85" s="33"/>
+      <c r="P85" s="20"/>
+      <c r="Q85" s="20"/>
+      <c r="R85" s="21"/>
+      <c r="S85" s="22"/>
+      <c r="T85" s="23"/>
     </row>
     <row r="86" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="16"/>
@@ -2664,11 +2664,11 @@
       <c r="M86" s="7"/>
       <c r="N86" s="11"/>
       <c r="O86" s="10"/>
-      <c r="P86" s="30"/>
-      <c r="Q86" s="30"/>
-      <c r="R86" s="31"/>
-      <c r="S86" s="32"/>
-      <c r="T86" s="33"/>
+      <c r="P86" s="20"/>
+      <c r="Q86" s="20"/>
+      <c r="R86" s="21"/>
+      <c r="S86" s="22"/>
+      <c r="T86" s="23"/>
     </row>
     <row r="87" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
@@ -2686,11 +2686,11 @@
       <c r="M87" s="7"/>
       <c r="N87" s="11"/>
       <c r="O87" s="10"/>
-      <c r="P87" s="30"/>
-      <c r="Q87" s="30"/>
-      <c r="R87" s="31"/>
-      <c r="S87" s="32"/>
-      <c r="T87" s="33"/>
+      <c r="P87" s="20"/>
+      <c r="Q87" s="20"/>
+      <c r="R87" s="21"/>
+      <c r="S87" s="22"/>
+      <c r="T87" s="23"/>
     </row>
     <row r="88" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
@@ -2708,11 +2708,11 @@
       <c r="M88" s="7"/>
       <c r="N88" s="11"/>
       <c r="O88" s="10"/>
-      <c r="P88" s="30"/>
-      <c r="Q88" s="30"/>
-      <c r="R88" s="31"/>
-      <c r="S88" s="32"/>
-      <c r="T88" s="33"/>
+      <c r="P88" s="20"/>
+      <c r="Q88" s="20"/>
+      <c r="R88" s="21"/>
+      <c r="S88" s="22"/>
+      <c r="T88" s="23"/>
     </row>
     <row r="89" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
@@ -2730,11 +2730,11 @@
       <c r="M89" s="7"/>
       <c r="N89" s="11"/>
       <c r="O89" s="10"/>
-      <c r="P89" s="30"/>
-      <c r="Q89" s="30"/>
-      <c r="R89" s="31"/>
-      <c r="S89" s="32"/>
-      <c r="T89" s="33"/>
+      <c r="P89" s="20"/>
+      <c r="Q89" s="20"/>
+      <c r="R89" s="21"/>
+      <c r="S89" s="22"/>
+      <c r="T89" s="23"/>
     </row>
     <row r="90" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
@@ -2752,11 +2752,11 @@
       <c r="M90" s="7"/>
       <c r="N90" s="11"/>
       <c r="O90" s="10"/>
-      <c r="P90" s="30"/>
-      <c r="Q90" s="30"/>
-      <c r="R90" s="31"/>
-      <c r="S90" s="32"/>
-      <c r="T90" s="33"/>
+      <c r="P90" s="20"/>
+      <c r="Q90" s="20"/>
+      <c r="R90" s="21"/>
+      <c r="S90" s="22"/>
+      <c r="T90" s="23"/>
     </row>
     <row r="91" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="19"/>
@@ -2774,11 +2774,11 @@
       <c r="M91" s="7"/>
       <c r="N91" s="11"/>
       <c r="O91" s="10"/>
-      <c r="P91" s="30"/>
-      <c r="Q91" s="30"/>
-      <c r="R91" s="31"/>
-      <c r="S91" s="32"/>
-      <c r="T91" s="33"/>
+      <c r="P91" s="20"/>
+      <c r="Q91" s="20"/>
+      <c r="R91" s="21"/>
+      <c r="S91" s="22"/>
+      <c r="T91" s="23"/>
     </row>
     <row r="92" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="19"/>
@@ -2796,11 +2796,11 @@
       <c r="M92" s="7"/>
       <c r="N92" s="11"/>
       <c r="O92" s="10"/>
-      <c r="P92" s="30"/>
-      <c r="Q92" s="30"/>
-      <c r="R92" s="31"/>
-      <c r="S92" s="32"/>
-      <c r="T92" s="33"/>
+      <c r="P92" s="20"/>
+      <c r="Q92" s="20"/>
+      <c r="R92" s="21"/>
+      <c r="S92" s="22"/>
+      <c r="T92" s="23"/>
     </row>
     <row r="93" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="19"/>
@@ -2818,11 +2818,11 @@
       <c r="M93" s="7"/>
       <c r="N93" s="11"/>
       <c r="O93" s="10"/>
-      <c r="P93" s="30"/>
-      <c r="Q93" s="30"/>
-      <c r="R93" s="31"/>
-      <c r="S93" s="32"/>
-      <c r="T93" s="33"/>
+      <c r="P93" s="20"/>
+      <c r="Q93" s="20"/>
+      <c r="R93" s="21"/>
+      <c r="S93" s="22"/>
+      <c r="T93" s="23"/>
     </row>
     <row r="94" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="19"/>
@@ -2840,11 +2840,11 @@
       <c r="M94" s="7"/>
       <c r="N94" s="11"/>
       <c r="O94" s="10"/>
-      <c r="P94" s="30"/>
-      <c r="Q94" s="30"/>
-      <c r="R94" s="31"/>
-      <c r="S94" s="32"/>
-      <c r="T94" s="33"/>
+      <c r="P94" s="20"/>
+      <c r="Q94" s="20"/>
+      <c r="R94" s="21"/>
+      <c r="S94" s="22"/>
+      <c r="T94" s="23"/>
     </row>
     <row r="95" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="19"/>
@@ -2862,11 +2862,11 @@
       <c r="M95" s="7"/>
       <c r="N95" s="11"/>
       <c r="O95" s="10"/>
-      <c r="P95" s="30"/>
-      <c r="Q95" s="30"/>
-      <c r="R95" s="31"/>
-      <c r="S95" s="32"/>
-      <c r="T95" s="33"/>
+      <c r="P95" s="20"/>
+      <c r="Q95" s="20"/>
+      <c r="R95" s="21"/>
+      <c r="S95" s="22"/>
+      <c r="T95" s="23"/>
     </row>
     <row r="96" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
@@ -2884,11 +2884,11 @@
       <c r="M96" s="7"/>
       <c r="N96" s="11"/>
       <c r="O96" s="10"/>
-      <c r="P96" s="30"/>
-      <c r="Q96" s="30"/>
-      <c r="R96" s="31"/>
-      <c r="S96" s="32"/>
-      <c r="T96" s="33"/>
+      <c r="P96" s="20"/>
+      <c r="Q96" s="20"/>
+      <c r="R96" s="21"/>
+      <c r="S96" s="22"/>
+      <c r="T96" s="23"/>
     </row>
     <row r="97" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="19"/>
@@ -2906,11 +2906,11 @@
       <c r="M97" s="7"/>
       <c r="N97" s="11"/>
       <c r="O97" s="10"/>
-      <c r="P97" s="30"/>
-      <c r="Q97" s="30"/>
-      <c r="R97" s="31"/>
-      <c r="S97" s="32"/>
-      <c r="T97" s="33"/>
+      <c r="P97" s="20"/>
+      <c r="Q97" s="20"/>
+      <c r="R97" s="21"/>
+      <c r="S97" s="22"/>
+      <c r="T97" s="23"/>
     </row>
     <row r="98" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="19"/>
@@ -2928,11 +2928,11 @@
       <c r="M98" s="7"/>
       <c r="N98" s="11"/>
       <c r="O98" s="10"/>
-      <c r="P98" s="30"/>
-      <c r="Q98" s="30"/>
-      <c r="R98" s="31"/>
-      <c r="S98" s="32"/>
-      <c r="T98" s="33"/>
+      <c r="P98" s="20"/>
+      <c r="Q98" s="20"/>
+      <c r="R98" s="21"/>
+      <c r="S98" s="22"/>
+      <c r="T98" s="23"/>
     </row>
     <row r="99" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="19"/>
@@ -2950,11 +2950,11 @@
       <c r="M99" s="7"/>
       <c r="N99" s="11"/>
       <c r="O99" s="10"/>
-      <c r="P99" s="30"/>
-      <c r="Q99" s="30"/>
-      <c r="R99" s="31"/>
-      <c r="S99" s="32"/>
-      <c r="T99" s="33"/>
+      <c r="P99" s="20"/>
+      <c r="Q99" s="20"/>
+      <c r="R99" s="21"/>
+      <c r="S99" s="22"/>
+      <c r="T99" s="23"/>
     </row>
     <row r="100" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="19"/>
@@ -2972,11 +2972,11 @@
       <c r="M100" s="7"/>
       <c r="N100" s="11"/>
       <c r="O100" s="10"/>
-      <c r="P100" s="30"/>
-      <c r="Q100" s="30"/>
-      <c r="R100" s="31"/>
-      <c r="S100" s="32"/>
-      <c r="T100" s="33"/>
+      <c r="P100" s="20"/>
+      <c r="Q100" s="20"/>
+      <c r="R100" s="21"/>
+      <c r="S100" s="22"/>
+      <c r="T100" s="23"/>
     </row>
     <row r="101" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="19"/>
@@ -2994,11 +2994,11 @@
       <c r="M101" s="7"/>
       <c r="N101" s="11"/>
       <c r="O101" s="10"/>
-      <c r="P101" s="30"/>
-      <c r="Q101" s="30"/>
-      <c r="R101" s="31"/>
-      <c r="S101" s="32"/>
-      <c r="T101" s="33"/>
+      <c r="P101" s="20"/>
+      <c r="Q101" s="20"/>
+      <c r="R101" s="21"/>
+      <c r="S101" s="22"/>
+      <c r="T101" s="23"/>
     </row>
     <row r="102" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="19"/>
@@ -3016,11 +3016,11 @@
       <c r="M102" s="7"/>
       <c r="N102" s="11"/>
       <c r="O102" s="10"/>
-      <c r="P102" s="30"/>
-      <c r="Q102" s="30"/>
-      <c r="R102" s="31"/>
-      <c r="S102" s="32"/>
-      <c r="T102" s="33"/>
+      <c r="P102" s="20"/>
+      <c r="Q102" s="20"/>
+      <c r="R102" s="21"/>
+      <c r="S102" s="22"/>
+      <c r="T102" s="23"/>
     </row>
     <row r="103" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="19"/>
@@ -3038,11 +3038,11 @@
       <c r="M103" s="7"/>
       <c r="N103" s="11"/>
       <c r="O103" s="10"/>
-      <c r="P103" s="30"/>
-      <c r="Q103" s="30"/>
-      <c r="R103" s="31"/>
-      <c r="S103" s="32"/>
-      <c r="T103" s="33"/>
+      <c r="P103" s="20"/>
+      <c r="Q103" s="20"/>
+      <c r="R103" s="21"/>
+      <c r="S103" s="22"/>
+      <c r="T103" s="23"/>
     </row>
     <row r="104" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="19"/>
@@ -3060,11 +3060,11 @@
       <c r="M104" s="7"/>
       <c r="N104" s="11"/>
       <c r="O104" s="10"/>
-      <c r="P104" s="30"/>
-      <c r="Q104" s="30"/>
-      <c r="R104" s="31"/>
-      <c r="S104" s="32"/>
-      <c r="T104" s="33"/>
+      <c r="P104" s="20"/>
+      <c r="Q104" s="20"/>
+      <c r="R104" s="21"/>
+      <c r="S104" s="22"/>
+      <c r="T104" s="23"/>
     </row>
     <row r="105" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="19"/>
@@ -3082,11 +3082,11 @@
       <c r="M105" s="7"/>
       <c r="N105" s="11"/>
       <c r="O105" s="10"/>
-      <c r="P105" s="30"/>
-      <c r="Q105" s="30"/>
-      <c r="R105" s="31"/>
-      <c r="S105" s="32"/>
-      <c r="T105" s="33"/>
+      <c r="P105" s="20"/>
+      <c r="Q105" s="20"/>
+      <c r="R105" s="21"/>
+      <c r="S105" s="22"/>
+      <c r="T105" s="23"/>
     </row>
     <row r="106" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="19"/>
@@ -3104,11 +3104,11 @@
       <c r="M106" s="7"/>
       <c r="N106" s="11"/>
       <c r="O106" s="10"/>
-      <c r="P106" s="30"/>
-      <c r="Q106" s="30"/>
-      <c r="R106" s="31"/>
-      <c r="S106" s="32"/>
-      <c r="T106" s="33"/>
+      <c r="P106" s="20"/>
+      <c r="Q106" s="20"/>
+      <c r="R106" s="21"/>
+      <c r="S106" s="22"/>
+      <c r="T106" s="23"/>
     </row>
     <row r="107" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="19"/>
@@ -3126,11 +3126,11 @@
       <c r="M107" s="7"/>
       <c r="N107" s="11"/>
       <c r="O107" s="10"/>
-      <c r="P107" s="30"/>
-      <c r="Q107" s="30"/>
-      <c r="R107" s="31"/>
-      <c r="S107" s="32"/>
-      <c r="T107" s="33"/>
+      <c r="P107" s="20"/>
+      <c r="Q107" s="20"/>
+      <c r="R107" s="21"/>
+      <c r="S107" s="22"/>
+      <c r="T107" s="23"/>
     </row>
     <row r="108" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T108" s="4"/>
@@ -5243,6 +5243,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="A2:T2"/>
     <mergeCell ref="A3:T3"/>
@@ -5259,10 +5263,6 @@
     <mergeCell ref="P7:T7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>